<commit_message>
Updated to handle MVN dependency management
</commit_message>
<xml_diff>
--- a/mavenDependencyCollector/toplevelDependencies.xlsx
+++ b/mavenDependencyCollector/toplevelDependencies.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>groupID</t>
   </si>
@@ -26,52 +26,34 @@
     <t>scope</t>
   </si>
   <si>
-    <t>org.mapstruct</t>
+    <t>org.springframework.boot</t>
   </si>
   <si>
-    <t>mapstruct-jdk8</t>
+    <t>spring-boot-starter-jersey</t>
+  </si>
+  <si>
+    <t>2.2.2</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>org.liquibase</t>
+    <t>org.mongodb</t>
   </si>
   <si>
-    <t>liquibase-core</t>
+    <t>mongodb-driver</t>
   </si>
   <si>
-    <t>com.google.guava</t>
+    <t>0.0.1</t>
   </si>
   <si>
-    <t>guava</t>
+    <t>spring-boot-starter-data-mongodb</t>
   </si>
   <si>
-    <t>com.google.code.findbugs</t>
+    <t>3.3.3</t>
   </si>
   <si>
-    <t>jsr305</t>
-  </si>
-  <si>
-    <t>org.springframework.boot</t>
-  </si>
-  <si>
-    <t>spring-boot-starter-security</t>
-  </si>
-  <si>
-    <t>org.postgresql</t>
-  </si>
-  <si>
-    <t>postgresql</t>
-  </si>
-  <si>
-    <t>spring-boot-starter-tomcat</t>
-  </si>
-  <si>
-    <t>org.springframework.retry</t>
-  </si>
-  <si>
-    <t>spring-retry</t>
+    <t>spring-boot-starter-web</t>
   </si>
 </sst>
 </file>
@@ -147,105 +129,49 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>